<commit_message>
add levels to ordered categorical variables
</commit_message>
<xml_diff>
--- a/inst/extdata/waterpoints.xlsx
+++ b/inst/extdata/waterpoints.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -134,12 +134,6 @@
     <t xml:space="preserve">tap</t>
   </si>
   <si>
-    <t xml:space="preserve">safe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unsafe</t>
-  </si>
-  <si>
     <t xml:space="preserve">customers_use_2-liter_bucket_for_bathing,_per-liter_prices_increase_by_33%</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t xml:space="preserve">possibly_unsafe</t>
   </si>
   <si>
-    <t xml:space="preserve">probably_unsafe</t>
-  </si>
-  <si>
     <t xml:space="preserve">member(s)_of_owner_household,employee(s)</t>
   </si>
   <si>
@@ -170,13 +161,10 @@
     <t xml:space="preserve">storage_tank</t>
   </si>
   <si>
+    <t xml:space="preserve">public_sale_of_water,_bathing,_toilet</t>
+  </si>
+  <si>
     <t xml:space="preserve">possibly_safe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">public_sale_of_water,_bathing,_toilet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">probably_safe</t>
   </si>
   <si>
     <t xml:space="preserve">public_sale_of_water</t>
@@ -727,18 +715,14 @@
       <c r="Z2" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA2" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA2"/>
       <c r="AB2" t="n">
         <v>100</v>
       </c>
       <c r="AC2" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD2" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD2"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -798,7 +782,7 @@
         <v>0.16</v>
       </c>
       <c r="U3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V3" t="b">
         <v>1</v>
@@ -815,18 +799,14 @@
       <c r="Z3" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA3"/>
       <c r="AB3" t="n">
         <v>100</v>
       </c>
       <c r="AC3" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD3" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD3"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -856,7 +836,7 @@
         <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L4" t="n">
         <v>600</v>
@@ -868,7 +848,7 @@
         <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P4"/>
       <c r="Q4" t="n">
@@ -899,18 +879,14 @@
       <c r="Z4" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA4" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA4"/>
       <c r="AB4" t="n">
         <v>13.6</v>
       </c>
       <c r="AC4" t="n">
         <v>83.06</v>
       </c>
-      <c r="AD4" t="s">
-        <v>45</v>
-      </c>
+      <c r="AD4"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -940,7 +916,7 @@
         <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L5" t="n">
         <v>8000</v>
@@ -968,7 +944,7 @@
         <v>0.25</v>
       </c>
       <c r="U5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V5" t="b">
         <v>0</v>
@@ -985,9 +961,7 @@
       <c r="Z5" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA5" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA5"/>
       <c r="AB5" t="n">
         <v>48.3</v>
       </c>
@@ -995,7 +969,7 @@
         <v>351.91</v>
       </c>
       <c r="AD5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -1026,7 +1000,7 @@
         <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L6" t="n">
         <v>300</v>
@@ -1069,18 +1043,14 @@
       <c r="Z6" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA6" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA6"/>
       <c r="AB6" t="n">
         <v>100</v>
       </c>
       <c r="AC6" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD6" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD6"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1110,7 +1080,7 @@
         <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L7" t="n">
         <v>800</v>
@@ -1134,7 +1104,7 @@
         <v>0.04</v>
       </c>
       <c r="U7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V7" t="b">
         <v>1</v>
@@ -1149,18 +1119,14 @@
       <c r="Z7" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA7" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA7"/>
       <c r="AB7" t="n">
         <v>100</v>
       </c>
       <c r="AC7" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD7" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD7"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1190,7 +1156,7 @@
         <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -1202,7 +1168,7 @@
         <v>36</v>
       </c>
       <c r="O8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P8"/>
       <c r="Q8" t="n">
@@ -1216,7 +1182,7 @@
         <v>0.04</v>
       </c>
       <c r="U8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="V8" t="b">
         <v>1</v>
@@ -1233,18 +1199,14 @@
       <c r="Z8" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA8" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA8"/>
       <c r="AB8" t="n">
         <v>100</v>
       </c>
       <c r="AC8" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD8" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD8"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1274,7 +1236,7 @@
         <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L9" t="n">
         <v>8000</v>
@@ -1304,7 +1266,7 @@
         <v>0.23</v>
       </c>
       <c r="U9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V9" t="b">
         <v>1</v>
@@ -1321,18 +1283,14 @@
       <c r="Z9" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA9" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA9"/>
       <c r="AB9" t="n">
         <v>100</v>
       </c>
       <c r="AC9" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD9" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD9"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1362,7 +1320,7 @@
         <v>34</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L10" t="n">
         <v>6000</v>
@@ -1388,7 +1346,7 @@
         <v>0.07</v>
       </c>
       <c r="U10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V10" t="b">
         <v>0</v>
@@ -1397,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y10" t="n">
         <v>0</v>
@@ -1405,18 +1363,14 @@
       <c r="Z10" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA10"/>
       <c r="AB10" t="n">
         <v>100</v>
       </c>
       <c r="AC10" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD10" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD10"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1446,7 +1400,7 @@
         <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L11" t="n">
         <v>500</v>
@@ -1491,18 +1445,14 @@
       <c r="Z11" t="n">
         <v>22.75</v>
       </c>
-      <c r="AA11" t="s">
-        <v>52</v>
-      </c>
+      <c r="AA11"/>
       <c r="AB11" t="n">
         <v>100</v>
       </c>
       <c r="AC11" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD11" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD11"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1532,7 +1482,7 @@
         <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L12" t="n">
         <v>8000</v>
@@ -1544,7 +1494,7 @@
         <v>36</v>
       </c>
       <c r="O12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P12" t="n">
         <v>3</v>
@@ -1560,7 +1510,7 @@
         <v>0.09</v>
       </c>
       <c r="U12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V12" t="b">
         <v>0</v>
@@ -1569,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="X12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
@@ -1577,18 +1527,14 @@
       <c r="Z12" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA12" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA12"/>
       <c r="AB12" t="n">
         <v>100</v>
       </c>
       <c r="AC12" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD12" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD12"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1618,7 +1564,7 @@
         <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L13" t="n">
         <v>10000</v>
@@ -1648,14 +1594,14 @@
         <v>0.16</v>
       </c>
       <c r="U13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V13" t="b">
         <v>0</v>
       </c>
       <c r="W13"/>
       <c r="X13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
@@ -1663,9 +1609,7 @@
       <c r="Z13" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA13" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA13"/>
       <c r="AB13" t="n">
         <v>48.3</v>
       </c>
@@ -1673,7 +1617,7 @@
         <v>351.91</v>
       </c>
       <c r="AD13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
@@ -1687,7 +1631,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -1704,7 +1648,7 @@
         <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L14" t="n">
         <v>3000</v>
@@ -1734,7 +1678,7 @@
         <v>0.28</v>
       </c>
       <c r="U14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V14" t="b">
         <v>0</v>
@@ -1751,18 +1695,14 @@
       <c r="Z14" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA14" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA14"/>
       <c r="AB14" t="n">
         <v>100</v>
       </c>
       <c r="AC14" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD14" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD14"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1792,7 +1732,7 @@
         <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L15" t="n">
         <v>27000</v>
@@ -1822,7 +1762,7 @@
         <v>0.25</v>
       </c>
       <c r="U15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V15" t="b">
         <v>1</v>
@@ -1910,7 +1850,7 @@
         <v>7.81</v>
       </c>
       <c r="AA16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AB16" t="n">
         <v>100</v>
@@ -1918,9 +1858,7 @@
       <c r="AC16" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD16" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD16"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1933,7 +1871,7 @@
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -1950,7 +1888,7 @@
         <v>34</v>
       </c>
       <c r="K17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L17" t="n">
         <v>5000</v>
@@ -1977,7 +1915,7 @@
       <c r="V17"/>
       <c r="W17"/>
       <c r="X17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y17" t="n">
         <v>0</v>
@@ -1985,18 +1923,14 @@
       <c r="Z17" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA17" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA17"/>
       <c r="AB17" t="n">
         <v>100</v>
       </c>
       <c r="AC17" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD17" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD17"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2054,7 +1988,7 @@
         <v>0.11</v>
       </c>
       <c r="U18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="V18" t="b">
         <v>0</v>
@@ -2069,45 +2003,41 @@
       <c r="Z18" t="n">
         <v>16.87</v>
       </c>
-      <c r="AA18" t="s">
-        <v>52</v>
-      </c>
+      <c r="AA18"/>
       <c r="AB18" t="n">
         <v>100</v>
       </c>
       <c r="AC18" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD18" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD18"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
         <v>55</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
       </c>
       <c r="F19"/>
       <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I19"/>
       <c r="J19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K19" t="s">
         <v>35</v>
@@ -2151,9 +2081,7 @@
       <c r="Z19" t="n">
         <v>37.68</v>
       </c>
-      <c r="AA19" t="s">
-        <v>52</v>
-      </c>
+      <c r="AA19"/>
       <c r="AB19" t="n">
         <v>48.3</v>
       </c>
@@ -2161,7 +2089,7 @@
         <v>351.91</v>
       </c>
       <c r="AD19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
@@ -2169,23 +2097,23 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
       </c>
       <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
         <v>55</v>
-      </c>
-      <c r="E20" t="s">
-        <v>59</v>
       </c>
       <c r="F20"/>
       <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I20"/>
       <c r="J20" t="s">
@@ -2201,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O20" t="s">
         <v>37</v>
@@ -2235,41 +2163,37 @@
       <c r="Z20" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA20" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA20"/>
       <c r="AB20" t="n">
         <v>100</v>
       </c>
       <c r="AC20" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD20" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD20"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
       </c>
       <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
         <v>55</v>
-      </c>
-      <c r="E21" t="s">
-        <v>59</v>
       </c>
       <c r="F21"/>
       <c r="G21" t="b">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I21"/>
       <c r="J21" t="s">
@@ -2283,7 +2207,7 @@
       </c>
       <c r="M21"/>
       <c r="N21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O21"/>
       <c r="P21"/>
@@ -2297,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="X21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y21" t="n">
         <v>100</v>
@@ -2305,31 +2229,27 @@
       <c r="Z21" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA21" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA21"/>
       <c r="AB21" t="n">
         <v>100</v>
       </c>
       <c r="AC21" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD21" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD21"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -2387,41 +2307,37 @@
       <c r="Z22" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA22" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA22"/>
       <c r="AB22" t="n">
         <v>100</v>
       </c>
       <c r="AC22" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD22" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD22"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
       </c>
       <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
         <v>55</v>
-      </c>
-      <c r="E23" t="s">
-        <v>59</v>
       </c>
       <c r="F23" t="n">
         <v>2015</v>
       </c>
       <c r="G23"/>
       <c r="H23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I23"/>
       <c r="J23" t="s">
@@ -2459,7 +2375,7 @@
       </c>
       <c r="W23"/>
       <c r="X23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y23" t="n">
         <v>100</v>
@@ -2467,31 +2383,27 @@
       <c r="Z23" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA23" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA23"/>
       <c r="AB23" t="n">
         <v>100</v>
       </c>
       <c r="AC23" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD23" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD23"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -2505,10 +2417,10 @@
       </c>
       <c r="I24"/>
       <c r="J24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L24" t="n">
         <v>800</v>
@@ -2517,7 +2429,7 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O24" t="s">
         <v>37</v>
@@ -2532,7 +2444,7 @@
         <v>0.05</v>
       </c>
       <c r="U24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="V24" t="b">
         <v>1</v>
@@ -2549,31 +2461,27 @@
       <c r="Z24" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA24" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA24"/>
       <c r="AB24" t="n">
         <v>100</v>
       </c>
       <c r="AC24" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD24" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD24"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -2597,7 +2505,7 @@
       </c>
       <c r="M25"/>
       <c r="N25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O25"/>
       <c r="P25"/>
@@ -2619,7 +2527,7 @@
         <v>0</v>
       </c>
       <c r="X25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Y25" t="n">
         <v>100</v>
@@ -2627,41 +2535,37 @@
       <c r="Z25" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA25" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA25"/>
       <c r="AB25" t="n">
         <v>100</v>
       </c>
       <c r="AC25" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD25" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD25"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
       </c>
       <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
         <v>55</v>
-      </c>
-      <c r="E26" t="s">
-        <v>59</v>
       </c>
       <c r="F26"/>
       <c r="G26" t="b">
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I26"/>
       <c r="J26" t="s">
@@ -2701,31 +2605,27 @@
       <c r="Z26" t="n">
         <v>2.87</v>
       </c>
-      <c r="AA26" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA26"/>
       <c r="AB26" t="n">
         <v>13.6</v>
       </c>
       <c r="AC26" t="n">
         <v>83.06</v>
       </c>
-      <c r="AD26" t="s">
-        <v>45</v>
-      </c>
+      <c r="AD26"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
         <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -2781,31 +2681,27 @@
       <c r="Z27" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA27" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA27"/>
       <c r="AB27" t="n">
         <v>100</v>
       </c>
       <c r="AC27" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD27" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD27"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
@@ -2831,10 +2727,10 @@
         <v>2</v>
       </c>
       <c r="N28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P28"/>
       <c r="Q28" t="n">
@@ -2848,7 +2744,7 @@
         <v>0.05</v>
       </c>
       <c r="U28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="V28" t="b">
         <v>1</v>
@@ -2857,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="X28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Y28" t="n">
         <v>4.7</v>
@@ -2865,41 +2761,37 @@
       <c r="Z28" t="n">
         <v>22.75</v>
       </c>
-      <c r="AA28" t="s">
-        <v>52</v>
-      </c>
+      <c r="AA28"/>
       <c r="AB28" t="n">
         <v>100</v>
       </c>
       <c r="AC28" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD28" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD28"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
         <v>31</v>
       </c>
       <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
         <v>55</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
       </c>
       <c r="F29"/>
       <c r="G29" t="b">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I29"/>
       <c r="J29" t="s">
@@ -2913,10 +2805,10 @@
       </c>
       <c r="M29"/>
       <c r="N29" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P29"/>
       <c r="Q29" t="n">
@@ -2937,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="X29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Y29" t="n">
         <v>48.3</v>
@@ -2946,7 +2838,7 @@
         <v>351.91</v>
       </c>
       <c r="AA29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AB29" t="n">
         <v>100</v>
@@ -2954,22 +2846,20 @@
       <c r="AC29" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD29" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD29"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
         <v>33</v>
@@ -3029,31 +2919,27 @@
       <c r="Z30" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA30" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA30"/>
       <c r="AB30" t="n">
         <v>100</v>
       </c>
       <c r="AC30" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD30" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD30"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
         <v>33</v>
@@ -3077,10 +2963,10 @@
       </c>
       <c r="M31"/>
       <c r="N31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P31"/>
       <c r="Q31" t="n">
@@ -3111,31 +2997,27 @@
       <c r="Z31" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA31" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA31"/>
       <c r="AB31" t="n">
         <v>100</v>
       </c>
       <c r="AC31" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD31" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD31"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
         <v>33</v>
@@ -3162,7 +3044,7 @@
         <v>36</v>
       </c>
       <c r="O32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P32"/>
       <c r="Q32" t="n">
@@ -3192,7 +3074,7 @@
         <v>6.64</v>
       </c>
       <c r="AA32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AB32" t="n">
         <v>100</v>
@@ -3200,25 +3082,23 @@
       <c r="AC32" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD32" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD32"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F33" t="n">
         <v>2005</v>
@@ -3242,7 +3122,7 @@
         <v>36</v>
       </c>
       <c r="O33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P33"/>
       <c r="Q33" t="n">
@@ -3271,34 +3151,30 @@
       <c r="Z33" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA33" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA33"/>
       <c r="AB33" t="n">
         <v>100</v>
       </c>
       <c r="AC33" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD33" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD33"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F34"/>
       <c r="G34" t="b">
@@ -3340,7 +3216,7 @@
         <v>0.14</v>
       </c>
       <c r="U34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="V34" t="b">
         <v>1</v>
@@ -3357,31 +3233,27 @@
       <c r="Z34" t="n">
         <v>22.75</v>
       </c>
-      <c r="AA34" t="s">
-        <v>52</v>
-      </c>
+      <c r="AA34"/>
       <c r="AB34" t="n">
         <v>100</v>
       </c>
       <c r="AC34" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD34" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD34"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s">
         <v>33</v>
@@ -3429,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="X35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y35" t="n">
         <v>100</v>
@@ -3437,34 +3309,30 @@
       <c r="Z35" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA35" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA35"/>
       <c r="AB35" t="n">
         <v>100</v>
       </c>
       <c r="AC35" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD35" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD35"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
         <v>31</v>
       </c>
       <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
         <v>55</v>
-      </c>
-      <c r="E36" t="s">
-        <v>59</v>
       </c>
       <c r="F36" t="n">
         <v>2017</v>
@@ -3517,34 +3385,30 @@
       <c r="Z36" t="n">
         <v>12.53</v>
       </c>
-      <c r="AA36" t="s">
-        <v>52</v>
-      </c>
+      <c r="AA36"/>
       <c r="AB36" t="n">
         <v>100</v>
       </c>
       <c r="AC36" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD36" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD36"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
         <v>31</v>
       </c>
       <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" t="s">
         <v>55</v>
-      </c>
-      <c r="E37" t="s">
-        <v>59</v>
       </c>
       <c r="F37" t="n">
         <v>2003</v>
@@ -3570,7 +3434,7 @@
         <v>36</v>
       </c>
       <c r="O37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P37"/>
       <c r="Q37" t="n">
@@ -3599,41 +3463,37 @@
       <c r="Z37" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA37" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA37"/>
       <c r="AB37" t="n">
         <v>100</v>
       </c>
       <c r="AC37" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD37" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD37"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
         <v>31</v>
       </c>
       <c r="D38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" t="s">
         <v>55</v>
-      </c>
-      <c r="E38" t="s">
-        <v>59</v>
       </c>
       <c r="F38" t="n">
         <v>1998</v>
       </c>
       <c r="G38"/>
       <c r="H38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I38"/>
       <c r="J38" t="s">
@@ -3650,7 +3510,7 @@
         <v>36</v>
       </c>
       <c r="O38" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P38"/>
       <c r="Q38" t="n">
@@ -3679,31 +3539,27 @@
       <c r="Z38" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA38" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA38"/>
       <c r="AB38" t="n">
         <v>100</v>
       </c>
       <c r="AC38" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD38" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD38"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E39" t="s">
         <v>33</v>
@@ -3732,7 +3588,7 @@
         <v>36</v>
       </c>
       <c r="O39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P39"/>
       <c r="Q39" t="n">
@@ -3755,7 +3611,7 @@
         <v>1</v>
       </c>
       <c r="X39" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y39" t="n">
         <v>48.3</v>
@@ -3764,7 +3620,7 @@
         <v>351.91</v>
       </c>
       <c r="AA39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AB39" t="n">
         <v>100</v>
@@ -3772,22 +3628,20 @@
       <c r="AC39" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD39" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD39"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
         <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E40" t="s">
         <v>33</v>
@@ -3814,7 +3668,7 @@
         <v>36</v>
       </c>
       <c r="O40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P40"/>
       <c r="Q40" t="n">
@@ -3841,31 +3695,27 @@
       <c r="Z40" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA40" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA40"/>
       <c r="AB40" t="n">
         <v>100</v>
       </c>
       <c r="AC40" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD40" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD40"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
         <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s">
         <v>33</v>
@@ -3894,7 +3744,7 @@
         <v>36</v>
       </c>
       <c r="O41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P41"/>
       <c r="Q41" t="n">
@@ -3908,7 +3758,7 @@
         <v>0.07</v>
       </c>
       <c r="U41" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="V41" t="b">
         <v>0</v>
@@ -3926,7 +3776,7 @@
         <v>351.91</v>
       </c>
       <c r="AA41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AB41" t="n">
         <v>100</v>
@@ -3934,16 +3784,14 @@
       <c r="AC41" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD41" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD41"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
         <v>31</v>
@@ -3978,7 +3826,7 @@
         <v>36</v>
       </c>
       <c r="O42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P42"/>
       <c r="Q42" t="n">
@@ -3994,7 +3842,7 @@
         <v>0.09</v>
       </c>
       <c r="U42" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="V42" t="b">
         <v>0</v>
@@ -4011,31 +3859,27 @@
       <c r="Z42" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA42" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA42"/>
       <c r="AB42" t="n">
         <v>100</v>
       </c>
       <c r="AC42" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD42" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD42"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
         <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E43" t="s">
         <v>33</v>
@@ -4064,7 +3908,7 @@
         <v>36</v>
       </c>
       <c r="O43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P43"/>
       <c r="Q43" t="n">
@@ -4095,31 +3939,27 @@
       <c r="Z43" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA43" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA43"/>
       <c r="AB43" t="n">
         <v>100</v>
       </c>
       <c r="AC43" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD43" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD43"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
         <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E44" t="s">
         <v>33</v>
@@ -4146,7 +3986,7 @@
         <v>36</v>
       </c>
       <c r="O44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P44"/>
       <c r="Q44" t="n">
@@ -4177,31 +4017,27 @@
       <c r="Z44" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA44" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA44"/>
       <c r="AB44" t="n">
         <v>100</v>
       </c>
       <c r="AC44" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD44" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD44"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
         <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E45" t="s">
         <v>33</v>
@@ -4228,7 +4064,7 @@
         <v>36</v>
       </c>
       <c r="O45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P45"/>
       <c r="Q45" t="n">
@@ -4255,34 +4091,30 @@
       <c r="Z45" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA45" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA45"/>
       <c r="AB45" t="n">
         <v>100</v>
       </c>
       <c r="AC45" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD45" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD45"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
         <v>31</v>
       </c>
       <c r="D46" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" t="s">
         <v>55</v>
-      </c>
-      <c r="E46" t="s">
-        <v>59</v>
       </c>
       <c r="F46" t="n">
         <v>2018</v>
@@ -4308,7 +4140,7 @@
         <v>36</v>
       </c>
       <c r="O46" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P46"/>
       <c r="Q46" t="n">
@@ -4329,7 +4161,7 @@
         <v>0</v>
       </c>
       <c r="X46" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y46" t="n">
         <v>13.6</v>
@@ -4337,34 +4169,30 @@
       <c r="Z46" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA46" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA46"/>
       <c r="AB46" t="n">
         <v>100</v>
       </c>
       <c r="AC46" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD46" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD46"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D47" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" t="s">
         <v>55</v>
-      </c>
-      <c r="E47" t="s">
-        <v>59</v>
       </c>
       <c r="F47"/>
       <c r="G47" t="b">
@@ -4376,17 +4204,17 @@
       </c>
       <c r="J47"/>
       <c r="K47" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L47" t="n">
         <v>0</v>
       </c>
       <c r="M47"/>
       <c r="N47" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P47"/>
       <c r="Q47" t="n">
@@ -4414,7 +4242,7 @@
         <v>145.55</v>
       </c>
       <c r="AA47" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AB47" t="n">
         <v>100</v>
@@ -4422,22 +4250,20 @@
       <c r="AC47" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD47" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD47"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
         <v>31</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E48" t="s">
         <v>33</v>
@@ -4487,34 +4313,30 @@
       <c r="Z48" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA48" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA48"/>
       <c r="AB48" t="n">
         <v>100</v>
       </c>
       <c r="AC48" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD48" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD48"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
         <v>31</v>
       </c>
       <c r="D49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" t="s">
         <v>55</v>
-      </c>
-      <c r="E49" t="s">
-        <v>59</v>
       </c>
       <c r="F49"/>
       <c r="G49"/>
@@ -4553,25 +4375,21 @@
       <c r="Z49" t="n">
         <v>83.06</v>
       </c>
-      <c r="AA49" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA49"/>
       <c r="AB49" t="n">
         <v>100</v>
       </c>
       <c r="AC49" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD49" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD49"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
         <v>31</v>
@@ -4580,14 +4398,14 @@
         <v>32</v>
       </c>
       <c r="E50" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F50" t="n">
         <v>2012</v>
       </c>
       <c r="G50"/>
       <c r="H50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I50"/>
       <c r="J50" t="s">
@@ -4606,7 +4424,7 @@
         <v>36</v>
       </c>
       <c r="O50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P50"/>
       <c r="Q50" t="n">
@@ -4620,7 +4438,7 @@
         <v>0.06</v>
       </c>
       <c r="U50" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="V50" t="b">
         <v>0</v>
@@ -4629,7 +4447,7 @@
         <v>0</v>
       </c>
       <c r="X50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y50" t="n">
         <v>100</v>
@@ -4637,18 +4455,14 @@
       <c r="Z50" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AA50" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA50"/>
       <c r="AB50" t="n">
         <v>100</v>
       </c>
       <c r="AC50" t="n">
         <v>9435.1</v>
       </c>
-      <c r="AD50" t="s">
-        <v>41</v>
-      </c>
+      <c r="AD50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>